<commit_message>
Updated 'class' column to 'classifier'
</commit_message>
<xml_diff>
--- a/public/sheets/upload_template.xlsx
+++ b/public/sheets/upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoshi\Desktop\1_classifiers\1_classifiers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evansavage/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92101B6B-9768-4DE6-B20E-C8DC142C30D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC756A7-CD27-244F-9FE7-497EA077E6BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27E08472-5E2E-4771-AE88-9F488C1AA2D8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{27E08472-5E2E-4771-AE88-9F488C1AA2D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -51,10 +48,10 @@
     <t>description</t>
   </si>
   <si>
-    <t>class</t>
-  </si>
-  <si>
     <t>encoding</t>
+  </si>
+  <si>
+    <t>classifier</t>
   </si>
 </sst>
 </file>
@@ -408,19 +405,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10780C14-38A1-424D-91A1-E73B4D8FF651}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="6" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -437,10 +435,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>